<commit_message>
updated dependencies and add excel / json field
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\ExcelParserExt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Excelparser\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0631D5E-29B3-40EF-BAFE-6FF4ABC93332}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="1272" yWindow="-96" windowWidth="21864" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Json" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>url</t>
   </si>
@@ -168,12 +169,21 @@
   </si>
   <si>
     <t>caption_de</t>
+  </si>
+  <si>
+    <t>sold</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -216,7 +226,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -493,25 +503,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" customWidth="1"/>
-    <col min="8" max="8" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.578125" customWidth="1"/>
+    <col min="2" max="2" width="17.578125" customWidth="1"/>
+    <col min="3" max="3" width="38.83984375" customWidth="1"/>
+    <col min="4" max="4" width="43.68359375" customWidth="1"/>
+    <col min="5" max="5" width="28.15625" customWidth="1"/>
+    <col min="7" max="7" width="28.578125" customWidth="1"/>
+    <col min="8" max="8" width="38.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,8 +549,11 @@
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -568,8 +581,11 @@
       <c r="I2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -597,8 +613,11 @@
       <c r="I3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -627,7 +646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -656,7 +675,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -685,7 +704,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -714,7 +733,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -743,7 +762,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -772,7 +791,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>39</v>
       </c>

</xml_diff>